<commit_message>
23rd August - drafting commit
</commit_message>
<xml_diff>
--- a/Results/PCA_Results_For_All_Wheat.xlsx
+++ b/Results/PCA_Results_For_All_Wheat.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Emmer and Einkorn" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Wild Emmer and Einkorn" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Einkorn" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Emmer" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Barley" sheetId="4" state="visible" r:id="rId4"/>
@@ -411,10 +411,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3806269531937028</v>
+        <v>0.3721544792316152</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2664575026527216</v>
+        <v>0.1043231789536628</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -422,10 +422,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2945167837357099</v>
+        <v>0.3508204786128634</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.8648896669172546</v>
+        <v>-0.7455931581521854</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -433,10 +433,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3943200280599</v>
+        <v>0.3526999915615989</v>
       </c>
       <c r="C4" t="n">
-        <v>0.414180957451828</v>
+        <v>0.6552583507526101</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -444,10 +444,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4537286854768851</v>
+        <v>0.4583657748124931</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.01517312220816891</v>
+        <v>-0.003291137479821626</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -455,10 +455,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4447775849991605</v>
+        <v>0.4399877922076786</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.07205947845148314</v>
+        <v>-0.05146209735416027</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -466,10 +466,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4573815496158807</v>
+        <v>0.4586287284011868</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06322662217673231</v>
+        <v>0.0344213824333387</v>
       </c>
     </row>
   </sheetData>
@@ -504,10 +504,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.4087576322602194</v>
+        <v>-0.4087576322602193</v>
       </c>
       <c r="C2" t="n">
-        <v>0.105936364969713</v>
+        <v>0.1059363649697134</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -515,10 +515,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2383853422796499</v>
+        <v>-0.2383853422796498</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.8704158396480774</v>
+        <v>-0.8704158396480776</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -526,10 +526,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.3798801081040959</v>
+        <v>-0.3798801081040958</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4719196994013412</v>
+        <v>0.4719196994013413</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -537,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.4600816232039394</v>
+        <v>-0.4600816232039395</v>
       </c>
       <c r="C5" t="n">
         <v>-0.03658881256473528</v>
@@ -548,10 +548,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4537686903103584</v>
+        <v>-0.4537686903103582</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0582714968126547</v>
+        <v>-0.05827149681265453</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -559,10 +559,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.4628170327527978</v>
+        <v>-0.4628170327527977</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06091995927444099</v>
+        <v>0.06091995927444105</v>
       </c>
     </row>
   </sheetData>
@@ -597,10 +597,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.4163999084396877</v>
+        <v>-0.4163999084396875</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.3013862094196736</v>
+        <v>-0.3013862094196741</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -608,10 +608,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.3087437282723046</v>
+        <v>-0.3087437282723052</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7228606580623401</v>
+        <v>0.7228606580623405</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -619,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.386647605923086</v>
+        <v>-0.3866476059230858</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4945255840539675</v>
+        <v>-0.4945255840539674</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -630,10 +630,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.4577488248650108</v>
+        <v>-0.4577488248650109</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.05135376020091392</v>
+        <v>-0.05135376020091403</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -641,10 +641,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4031956695964491</v>
+        <v>-0.4031956695964494</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3672247980680075</v>
+        <v>0.3672247980680073</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -652,10 +652,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.4579206489024668</v>
+        <v>-0.4579206489024669</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.06776435280102905</v>
+        <v>-0.06776435280102949</v>
       </c>
     </row>
   </sheetData>
@@ -690,10 +690,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3903008835525391</v>
+        <v>0.3903008835525389</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.412863934157771</v>
+        <v>-0.4128639341577707</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -701,10 +701,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2040553963386508</v>
+        <v>0.2040553963386507</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7310653254324938</v>
+        <v>0.731065325432493</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -712,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3595474228337251</v>
+        <v>0.3595474228337249</v>
       </c>
       <c r="C4" t="n">
         <v>-0.487758587974171</v>
@@ -723,10 +723,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4816467844222869</v>
+        <v>0.4816467844222868</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09964651911847844</v>
+        <v>0.09964651911847838</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -737,7 +737,7 @@
         <v>0.4622792341827735</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1880429904741637</v>
+        <v>0.1880429904741636</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -745,10 +745,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4806938224648518</v>
+        <v>0.4806938224648517</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1090358961104009</v>
+        <v>0.1090358961104006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I literally hate myself
</commit_message>
<xml_diff>
--- a/Results/PCA_Results_For_All_Wheat.xlsx
+++ b/Results/PCA_Results_For_All_Wheat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>PC-1</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>mean_surface_area</t>
-  </si>
-  <si>
-    <t>mean_length_depth_width</t>
   </si>
 </sst>
 </file>
@@ -390,7 +387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,10 +408,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3721544792316152</v>
+        <v>0.5115821815672132</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1043231789536628</v>
+        <v>0.02175819009777252</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -422,10 +419,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3508204786128634</v>
+        <v>0.4054111960378419</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7455931581521854</v>
+        <v>-0.7118471303185286</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -433,10 +430,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3526999915615989</v>
+        <v>0.4113086412639908</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6552583507526101</v>
+        <v>0.1341045258859178</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -444,10 +441,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4583657748124931</v>
+        <v>0.3901037336585669</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.003291137479821626</v>
+        <v>0.6834080668637618</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -455,21 +452,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4399877922076786</v>
+        <v>0.5025631425376446</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.05146209735416027</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.4586287284011868</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0344213824333387</v>
+        <v>-0.08814553025193195</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,10 +490,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.4087576322602193</v>
+        <v>-0.5186840863940005</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1059363649697134</v>
+        <v>-0.01520805295325373</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -515,10 +501,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2383853422796498</v>
+        <v>-0.2776044042943789</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.8704158396480776</v>
+        <v>-0.8610860848542273</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -526,10 +512,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.3798801081040958</v>
+        <v>-0.4606501046128745</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4719196994013413</v>
+        <v>0.1266835982382657</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -537,10 +523,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.4600816232039395</v>
+        <v>-0.4213634355599578</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.03658881256473528</v>
+        <v>0.4909035238897989</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -548,21 +534,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4537686903103582</v>
+        <v>-0.5139620117588853</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.05827149681265453</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
-        <v>-0.4628170327527977</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.06091995927444105</v>
+        <v>-0.03555932740888018</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,10 +572,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.4163999084396875</v>
+        <v>-0.5194204750270668</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.3013862094196741</v>
+        <v>-0.07806132019184023</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -608,10 +583,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.3087437282723052</v>
+        <v>-0.3448150747342947</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7228606580623405</v>
+        <v>0.6989225872624897</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -619,10 +594,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.3866476059230858</v>
+        <v>-0.4622486903490475</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4945255840539674</v>
+        <v>-0.3276280529488359</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -630,10 +605,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.4577488248650109</v>
+        <v>-0.4139741641828348</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.05135376020091403</v>
+        <v>-0.5233253765996744</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -641,21 +616,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4031956695964494</v>
+        <v>-0.4756642450493342</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3672247980680073</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
-        <v>-0.4579206489024669</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-0.06776435280102949</v>
+        <v>0.3524259587941533</v>
       </c>
     </row>
   </sheetData>
@@ -669,7 +633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -690,10 +654,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3903008835525389</v>
+        <v>-0.5660876030972491</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.4128639341577707</v>
+        <v>0.1083208302699449</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -701,10 +665,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2040553963386507</v>
+        <v>-0.1928640120986571</v>
       </c>
       <c r="C3" t="n">
-        <v>0.731065325432493</v>
+        <v>0.6946371660720148</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -712,10 +676,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3595474228337249</v>
+        <v>-0.4930486747734305</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.487758587974171</v>
+        <v>-0.3311659381744667</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -723,10 +687,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4816467844222868</v>
+        <v>-0.3827057494038196</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09964651911847838</v>
+        <v>-0.5298331396828329</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -734,21 +698,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4622792341827735</v>
+        <v>-0.5027798843770949</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1880429904741636</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.4806938224648517</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.1090358961104006</v>
+        <v>0.3396347607768182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>